<commit_message>
all files cleaned, 'Problematic' renamed
</commit_message>
<xml_diff>
--- a/labelled_csv_files/PROBLEMATIC_labelled_M_0104_10y3m_1_fa.xlsx
+++ b/labelled_csv_files/PROBLEMATIC_labelled_M_0104_10y3m_1_fa.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shababayub/go/src/github.com/s4ayub/fydp/labelled_csv_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahul/Documents/fydp/labelled_csv_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B8F0CE56-1BA1-5448-BDC2-788B997C521A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{795F617E-B53D-1544-9750-D096CFD67735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="11580" windowHeight="15000"/>
+    <workbookView xWindow="-21320" yWindow="-180" windowWidth="17940" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="labelled_M_0104_10y3m_1_fa" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="868" uniqueCount="498">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="868" uniqueCount="496">
   <si>
     <t>title</t>
   </si>
@@ -1512,19 +1520,13 @@
     <t>tone.</t>
   </si>
   <si>
-    <t>not aligned properly</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>comletely off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="12"/>
@@ -1661,17 +1663,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
@@ -2016,8 +2014,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2374,11 +2374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D274" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F287" sqref="F287"/>
+    <sheetView tabSelected="1" topLeftCell="B266" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E275" sqref="E275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2430,21 +2430,19 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>7.2350000000000003</v>
-      </c>
-      <c r="D3" s="1">
-        <v>9.3350000000000009</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="3">
+        <v>10.227</v>
+      </c>
+      <c r="D3" s="3">
+        <v>11.217000000000001</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>495</v>
-      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
@@ -2453,18 +2451,19 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
-        <v>9.3350000000000009</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10.225</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="3">
+        <v>12.076000000000001</v>
+      </c>
+      <c r="D4" s="3">
+        <v>12.170999999999999</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
@@ -2474,10 +2473,10 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>10.225</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>10.62</v>
+        <v>13.01</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -2494,10 +2493,10 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>10.62</v>
+        <v>13.05</v>
       </c>
       <c r="D6">
-        <v>10.775</v>
+        <v>13.1343</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -2594,10 +2593,10 @@
         <v>26</v>
       </c>
       <c r="C11">
-        <v>15.845000000000001</v>
+        <v>18.013999999999999</v>
       </c>
       <c r="D11">
-        <v>16.899999999999999</v>
+        <v>18.059999999999999</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
@@ -2654,10 +2653,10 @@
         <v>32</v>
       </c>
       <c r="C14">
-        <v>18.715</v>
+        <v>18.222999999999999</v>
       </c>
       <c r="D14">
-        <v>20.05</v>
+        <v>20.010000000000002</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -2674,10 +2673,10 @@
         <v>35</v>
       </c>
       <c r="C15">
-        <v>20.05</v>
+        <v>21.16</v>
       </c>
       <c r="D15">
-        <v>20.29</v>
+        <v>21.28</v>
       </c>
       <c r="E15" t="s">
         <v>36</v>
@@ -2694,10 +2693,10 @@
         <v>37</v>
       </c>
       <c r="C16">
-        <v>20.29</v>
+        <v>22.02</v>
       </c>
       <c r="D16">
-        <v>22.545000000000002</v>
+        <v>22.08</v>
       </c>
       <c r="E16" t="s">
         <v>38</v>
@@ -2774,10 +2773,10 @@
         <v>45</v>
       </c>
       <c r="C20">
-        <v>24.28</v>
+        <v>24.07</v>
       </c>
       <c r="D20">
-        <v>25.74</v>
+        <v>24.15</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
@@ -2854,10 +2853,10 @@
         <v>53</v>
       </c>
       <c r="C24">
-        <v>26.7</v>
+        <v>26.2</v>
       </c>
       <c r="D24">
-        <v>27.954999999999998</v>
+        <v>27.2</v>
       </c>
       <c r="E24" t="s">
         <v>54</v>
@@ -2914,16 +2913,16 @@
         <v>59</v>
       </c>
       <c r="C27">
-        <v>28.72</v>
+        <v>28.07</v>
       </c>
       <c r="D27">
-        <v>29.59</v>
+        <v>29.02</v>
       </c>
       <c r="E27" t="s">
         <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>496</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2974,10 +2973,10 @@
         <v>65</v>
       </c>
       <c r="C30">
-        <v>31.11</v>
+        <v>30.1</v>
       </c>
       <c r="D30">
-        <v>31.925000000000001</v>
+        <v>31.09</v>
       </c>
       <c r="E30" t="s">
         <v>66</v>
@@ -3054,10 +3053,10 @@
         <v>72</v>
       </c>
       <c r="C34">
-        <v>34.164999999999999</v>
+        <v>31.22</v>
       </c>
       <c r="D34">
-        <v>35.340000000000003</v>
+        <v>31.4</v>
       </c>
       <c r="E34" t="s">
         <v>73</v>
@@ -3074,10 +3073,10 @@
         <v>74</v>
       </c>
       <c r="C35">
-        <v>35.340000000000003</v>
+        <v>31.4</v>
       </c>
       <c r="D35">
-        <v>36.965000000000003</v>
+        <v>31.7</v>
       </c>
       <c r="E35" t="s">
         <v>73</v>
@@ -3094,10 +3093,10 @@
         <v>75</v>
       </c>
       <c r="C36">
-        <v>36.965000000000003</v>
+        <v>31.7</v>
       </c>
       <c r="D36">
-        <v>37.770000000000003</v>
+        <v>32.1</v>
       </c>
       <c r="E36" t="s">
         <v>76</v>
@@ -3114,10 +3113,10 @@
         <v>77</v>
       </c>
       <c r="C37">
-        <v>37.770000000000003</v>
+        <v>32.119999999999997</v>
       </c>
       <c r="D37">
-        <v>39.5</v>
+        <v>32.24</v>
       </c>
       <c r="E37" t="s">
         <v>78</v>
@@ -3134,10 +3133,10 @@
         <v>79</v>
       </c>
       <c r="C38">
-        <v>39.5</v>
+        <v>32.24</v>
       </c>
       <c r="D38">
-        <v>39.799999999999997</v>
+        <v>33.03</v>
       </c>
       <c r="E38" t="s">
         <v>76</v>
@@ -3154,10 +3153,10 @@
         <v>80</v>
       </c>
       <c r="C39">
-        <v>39.799999999999997</v>
+        <v>33.07</v>
       </c>
       <c r="D39">
-        <v>42.02</v>
+        <v>33.21</v>
       </c>
       <c r="E39" t="s">
         <v>81</v>
@@ -3174,10 +3173,10 @@
         <v>82</v>
       </c>
       <c r="C40">
-        <v>42.02</v>
+        <v>33.21</v>
       </c>
       <c r="D40">
-        <v>42.91</v>
+        <v>34.01</v>
       </c>
       <c r="E40" t="s">
         <v>76</v>
@@ -3214,10 +3213,10 @@
         <v>84</v>
       </c>
       <c r="C42">
-        <v>43.255000000000003</v>
+        <v>34.19</v>
       </c>
       <c r="D42">
-        <v>44.21</v>
+        <v>34.21</v>
       </c>
       <c r="E42" t="s">
         <v>85</v>
@@ -3234,10 +3233,10 @@
         <v>86</v>
       </c>
       <c r="C43">
-        <v>44.21</v>
+        <v>34.22</v>
       </c>
       <c r="D43">
-        <v>44.494999999999997</v>
+        <v>35.04</v>
       </c>
       <c r="E43" t="s">
         <v>38</v>
@@ -3274,10 +3273,10 @@
         <v>89</v>
       </c>
       <c r="C45">
-        <v>44.795000000000002</v>
+        <v>36.22</v>
       </c>
       <c r="D45">
-        <v>45.055</v>
+        <v>37.049999999999997</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
@@ -3294,10 +3293,10 @@
         <v>91</v>
       </c>
       <c r="C46">
-        <v>45.055</v>
+        <v>37.21</v>
       </c>
       <c r="D46">
-        <v>45.274999999999999</v>
+        <v>37.22</v>
       </c>
       <c r="E46" t="s">
         <v>92</v>
@@ -3314,10 +3313,10 @@
         <v>93</v>
       </c>
       <c r="C47">
-        <v>45.274999999999999</v>
+        <v>37.229999999999997</v>
       </c>
       <c r="D47">
-        <v>46.034999999999997</v>
+        <v>39.020000000000003</v>
       </c>
       <c r="E47" t="s">
         <v>94</v>
@@ -3334,10 +3333,10 @@
         <v>95</v>
       </c>
       <c r="C48">
-        <v>46.034999999999997</v>
+        <v>39.06</v>
       </c>
       <c r="D48">
-        <v>46.295000000000002</v>
+        <v>39.090000000000003</v>
       </c>
       <c r="E48" t="s">
         <v>96</v>
@@ -3394,10 +3393,10 @@
         <v>99</v>
       </c>
       <c r="C51">
-        <v>46.555</v>
+        <v>40.159999999999997</v>
       </c>
       <c r="D51">
-        <v>46.83</v>
+        <v>41.04</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
@@ -3433,18 +3432,19 @@
       <c r="B53" t="s">
         <v>102</v>
       </c>
-      <c r="C53">
-        <v>47.06</v>
-      </c>
-      <c r="D53" s="1">
-        <v>47.16</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="C53" s="3">
+        <v>42</v>
+      </c>
+      <c r="D53" s="3">
+        <v>42.07</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
@@ -3453,18 +3453,19 @@
       <c r="B54" t="s">
         <v>104</v>
       </c>
-      <c r="C54">
-        <v>47.16</v>
-      </c>
-      <c r="D54" s="1">
-        <v>47.19</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="C54" s="3">
+        <v>42.09</v>
+      </c>
+      <c r="D54" s="3">
+        <v>41.18</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
@@ -3473,18 +3474,19 @@
       <c r="B55" t="s">
         <v>106</v>
       </c>
-      <c r="C55">
-        <v>47.19</v>
-      </c>
-      <c r="D55" s="1">
-        <v>47.7</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="C55" s="3">
+        <v>42.2</v>
+      </c>
+      <c r="D55" s="3">
+        <v>43.04</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
@@ -3493,18 +3495,19 @@
       <c r="B56" t="s">
         <v>108</v>
       </c>
-      <c r="C56">
-        <v>47.7</v>
-      </c>
-      <c r="D56" s="1">
-        <v>48.42</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="C56" s="3">
+        <v>45.1</v>
+      </c>
+      <c r="D56" s="3">
+        <v>43.18</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
@@ -3513,21 +3516,19 @@
       <c r="B57" t="s">
         <v>110</v>
       </c>
-      <c r="C57">
-        <v>48.42</v>
-      </c>
-      <c r="D57" s="1">
-        <v>48.65</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="C57" s="3">
+        <v>44.04</v>
+      </c>
+      <c r="D57" s="3">
+        <v>44.18</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>497</v>
-      </c>
+      <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
@@ -3536,18 +3537,19 @@
       <c r="B58" t="s">
         <v>112</v>
       </c>
-      <c r="C58">
-        <v>48.65</v>
-      </c>
-      <c r="D58" s="1">
-        <v>49.03</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="C58" s="3">
+        <v>44.19</v>
+      </c>
+      <c r="D58" s="3">
+        <v>45.09</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
@@ -3556,18 +3558,19 @@
       <c r="B59" t="s">
         <v>114</v>
       </c>
-      <c r="C59">
-        <v>49.03</v>
-      </c>
-      <c r="D59" s="1">
-        <v>49.274999999999999</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="C59" s="3">
+        <v>45.1</v>
+      </c>
+      <c r="D59" s="3">
+        <v>45.15</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
@@ -3576,18 +3579,19 @@
       <c r="B60" t="s">
         <v>115</v>
       </c>
-      <c r="C60">
-        <v>49.274999999999999</v>
-      </c>
-      <c r="D60" s="1">
-        <v>49.484999999999999</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="C60" s="3">
+        <v>45.15</v>
+      </c>
+      <c r="D60" s="3">
+        <v>45.19</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
@@ -3596,18 +3600,19 @@
       <c r="B61" t="s">
         <v>117</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="3">
         <v>49.484999999999999</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="3">
         <v>49.645000000000003</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
@@ -3616,18 +3621,19 @@
       <c r="B62" t="s">
         <v>119</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="3">
         <v>49.645000000000003</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="3">
         <v>49.66</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F62" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
@@ -3637,15 +3643,15 @@
         <v>121</v>
       </c>
       <c r="C63">
-        <v>49.66</v>
-      </c>
-      <c r="D63" s="1">
-        <v>50.965000000000003</v>
-      </c>
-      <c r="E63" s="1" t="s">
+        <v>46.046999999999997</v>
+      </c>
+      <c r="D63" s="3">
+        <v>47.06</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3656,16 +3662,16 @@
       <c r="B64" t="s">
         <v>123</v>
       </c>
-      <c r="C64">
-        <v>50.965000000000003</v>
-      </c>
-      <c r="D64" s="1">
-        <v>51.354999999999997</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="C64" s="3">
+        <v>47.07</v>
+      </c>
+      <c r="D64" s="3">
+        <v>47.11</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3676,16 +3682,16 @@
       <c r="B65" t="s">
         <v>125</v>
       </c>
-      <c r="C65">
-        <v>51.354999999999997</v>
-      </c>
-      <c r="D65" s="1">
-        <v>52.134999999999998</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="C65" s="3">
+        <v>47.11</v>
+      </c>
+      <c r="D65" s="3">
+        <v>47.2</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3696,16 +3702,16 @@
       <c r="B66" t="s">
         <v>127</v>
       </c>
-      <c r="C66">
-        <v>52.134999999999998</v>
-      </c>
-      <c r="D66" s="1">
-        <v>54.23</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="C66" s="3">
+        <v>47.18</v>
+      </c>
+      <c r="D66" s="3">
+        <v>49.03</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3757,10 +3763,10 @@
         <v>132</v>
       </c>
       <c r="C69">
-        <v>54.695</v>
+        <v>50.16</v>
       </c>
       <c r="D69">
-        <v>54.695</v>
+        <v>51</v>
       </c>
       <c r="E69" t="s">
         <v>16</v>
@@ -3797,10 +3803,10 @@
         <v>135</v>
       </c>
       <c r="C71">
-        <v>54.7</v>
+        <v>51.02</v>
       </c>
       <c r="D71">
-        <v>55.585000000000001</v>
+        <v>52</v>
       </c>
       <c r="E71" t="s">
         <v>136</v>
@@ -3817,10 +3823,10 @@
         <v>137</v>
       </c>
       <c r="C72">
-        <v>55.585000000000001</v>
+        <v>52</v>
       </c>
       <c r="D72">
-        <v>57.484999999999999</v>
+        <v>52.21</v>
       </c>
       <c r="E72" t="s">
         <v>138</v>
@@ -3877,10 +3883,10 @@
         <v>142</v>
       </c>
       <c r="C75">
-        <v>58.445</v>
+        <v>54.05</v>
       </c>
       <c r="D75">
-        <v>58.774999999999999</v>
+        <v>54.2</v>
       </c>
       <c r="E75" t="s">
         <v>143</v>
@@ -3897,10 +3903,10 @@
         <v>144</v>
       </c>
       <c r="C76">
-        <v>58.774999999999999</v>
+        <v>54.2</v>
       </c>
       <c r="D76">
-        <v>59.18</v>
+        <v>54.5</v>
       </c>
       <c r="E76" t="s">
         <v>145</v>
@@ -3917,10 +3923,10 @@
         <v>146</v>
       </c>
       <c r="C77">
-        <v>59.18</v>
+        <v>54.56</v>
       </c>
       <c r="D77">
-        <v>59.5</v>
+        <v>54.7</v>
       </c>
       <c r="E77" t="s">
         <v>147</v>
@@ -3977,10 +3983,10 @@
         <v>150</v>
       </c>
       <c r="C80">
-        <v>61.905000000000001</v>
+        <v>53.8</v>
       </c>
       <c r="D80">
-        <v>64.5</v>
+        <v>55</v>
       </c>
       <c r="E80" t="s">
         <v>151</v>
@@ -3997,10 +4003,10 @@
         <v>152</v>
       </c>
       <c r="C81">
-        <v>64.5</v>
+        <v>56.2</v>
       </c>
       <c r="D81">
-        <v>64.64</v>
+        <v>56.6</v>
       </c>
       <c r="E81" t="s">
         <v>153</v>
@@ -4057,10 +4063,10 @@
         <v>156</v>
       </c>
       <c r="C84">
-        <v>64.885000000000005</v>
+        <v>58.3</v>
       </c>
       <c r="D84">
-        <v>66.349999999999994</v>
+        <v>59.1</v>
       </c>
       <c r="E84" t="s">
         <v>157</v>
@@ -4137,10 +4143,10 @@
         <v>162</v>
       </c>
       <c r="C88">
-        <v>67.760000000000005</v>
+        <v>59</v>
       </c>
       <c r="D88">
-        <v>68.144999999999996</v>
+        <v>59.13</v>
       </c>
       <c r="E88" t="s">
         <v>163</v>
@@ -4157,10 +4163,10 @@
         <v>164</v>
       </c>
       <c r="C89">
-        <v>68.144999999999996</v>
+        <v>59.13</v>
       </c>
       <c r="D89">
-        <v>68.760000000000005</v>
+        <v>60</v>
       </c>
       <c r="E89" t="s">
         <v>165</v>
@@ -4197,10 +4203,10 @@
         <v>168</v>
       </c>
       <c r="C91">
-        <v>70.045000000000002</v>
+        <v>60.2</v>
       </c>
       <c r="D91">
-        <v>71.819999999999993</v>
+        <v>61</v>
       </c>
       <c r="E91" t="s">
         <v>169</v>
@@ -4217,10 +4223,10 @@
         <v>170</v>
       </c>
       <c r="C92">
-        <v>71.819999999999993</v>
+        <v>61</v>
       </c>
       <c r="D92">
-        <v>73.055000000000007</v>
+        <v>61.3</v>
       </c>
       <c r="E92" t="s">
         <v>171</v>
@@ -4237,10 +4243,10 @@
         <v>172</v>
       </c>
       <c r="C93">
-        <v>73.055000000000007</v>
+        <v>61.3</v>
       </c>
       <c r="D93">
-        <v>73.430000000000007</v>
+        <v>61.5</v>
       </c>
       <c r="E93" t="s">
         <v>171</v>
@@ -4257,10 +4263,10 @@
         <v>173</v>
       </c>
       <c r="C94">
-        <v>73.430000000000007</v>
+        <v>61.5</v>
       </c>
       <c r="D94">
-        <v>73.67</v>
+        <v>62</v>
       </c>
       <c r="E94" t="s">
         <v>174</v>
@@ -4277,10 +4283,10 @@
         <v>175</v>
       </c>
       <c r="C95">
-        <v>73.67</v>
+        <v>62</v>
       </c>
       <c r="D95">
-        <v>75.27</v>
+        <v>62.3</v>
       </c>
       <c r="E95" t="s">
         <v>176</v>
@@ -4297,10 +4303,10 @@
         <v>177</v>
       </c>
       <c r="C96">
-        <v>75.27</v>
+        <v>64</v>
       </c>
       <c r="D96">
-        <v>75.775000000000006</v>
+        <v>64.3</v>
       </c>
       <c r="E96" t="s">
         <v>178</v>
@@ -4317,10 +4323,10 @@
         <v>179</v>
       </c>
       <c r="C97">
-        <v>75.775000000000006</v>
+        <v>64.3</v>
       </c>
       <c r="D97">
-        <v>76.515000000000001</v>
+        <v>64.8</v>
       </c>
       <c r="E97" t="s">
         <v>180</v>
@@ -4377,10 +4383,10 @@
         <v>183</v>
       </c>
       <c r="C100">
-        <v>76.569999999999993</v>
+        <v>65</v>
       </c>
       <c r="D100">
-        <v>78.504999999999995</v>
+        <v>65.7</v>
       </c>
       <c r="E100" t="s">
         <v>184</v>
@@ -4397,10 +4403,10 @@
         <v>185</v>
       </c>
       <c r="C101">
-        <v>78.504999999999995</v>
+        <v>66</v>
       </c>
       <c r="D101">
-        <v>78.66</v>
+        <v>66.3</v>
       </c>
       <c r="E101" t="s">
         <v>16</v>
@@ -4417,10 +4423,10 @@
         <v>186</v>
       </c>
       <c r="C102">
-        <v>78.66</v>
+        <v>67</v>
       </c>
       <c r="D102">
-        <v>78.680000000000007</v>
+        <v>67.5</v>
       </c>
       <c r="E102" t="s">
         <v>178</v>
@@ -4437,10 +4443,10 @@
         <v>187</v>
       </c>
       <c r="C103">
-        <v>78.680000000000007</v>
+        <v>67.5</v>
       </c>
       <c r="D103">
-        <v>78.69</v>
+        <v>69.8</v>
       </c>
       <c r="E103" t="s">
         <v>178</v>
@@ -4517,10 +4523,10 @@
         <v>194</v>
       </c>
       <c r="C107">
-        <v>80.31</v>
+        <v>71</v>
       </c>
       <c r="D107">
-        <v>80.53</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="E107" t="s">
         <v>16</v>
@@ -4557,10 +4563,10 @@
         <v>197</v>
       </c>
       <c r="C109">
-        <v>80.61</v>
+        <v>72</v>
       </c>
       <c r="D109">
-        <v>82.46</v>
+        <v>73</v>
       </c>
       <c r="E109" t="s">
         <v>198</v>
@@ -4617,10 +4623,10 @@
         <v>203</v>
       </c>
       <c r="C112">
-        <v>83.02</v>
+        <v>76</v>
       </c>
       <c r="D112">
-        <v>86.305000000000007</v>
+        <v>76.75</v>
       </c>
       <c r="E112" t="s">
         <v>204</v>
@@ -4637,10 +4643,10 @@
         <v>205</v>
       </c>
       <c r="C113">
-        <v>86.305000000000007</v>
+        <v>77</v>
       </c>
       <c r="D113">
-        <v>86.465000000000003</v>
+        <v>77.2</v>
       </c>
       <c r="E113" t="s">
         <v>206</v>
@@ -4657,10 +4663,10 @@
         <v>207</v>
       </c>
       <c r="C114">
-        <v>86.465000000000003</v>
+        <v>77.2</v>
       </c>
       <c r="D114">
-        <v>86.48</v>
+        <v>78</v>
       </c>
       <c r="E114" t="s">
         <v>208</v>
@@ -4677,10 +4683,10 @@
         <v>209</v>
       </c>
       <c r="C115">
-        <v>86.48</v>
+        <v>78.06</v>
       </c>
       <c r="D115">
-        <v>86.495000000000005</v>
+        <v>78.2</v>
       </c>
       <c r="E115" t="s">
         <v>178</v>
@@ -4697,10 +4703,10 @@
         <v>210</v>
       </c>
       <c r="C116">
-        <v>86.495000000000005</v>
+        <v>79</v>
       </c>
       <c r="D116">
-        <v>86.495000000000005</v>
+        <v>79.5</v>
       </c>
       <c r="E116" t="s">
         <v>178</v>
@@ -4717,10 +4723,10 @@
         <v>211</v>
       </c>
       <c r="C117">
-        <v>86.495000000000005</v>
+        <v>79.5</v>
       </c>
       <c r="D117">
-        <v>86.594999999999999</v>
+        <v>79.75</v>
       </c>
       <c r="E117" t="s">
         <v>178</v>
@@ -4737,10 +4743,10 @@
         <v>212</v>
       </c>
       <c r="C118">
-        <v>86.594999999999999</v>
+        <v>79.75</v>
       </c>
       <c r="D118">
-        <v>86.734999999999999</v>
+        <v>79.8</v>
       </c>
       <c r="E118" t="s">
         <v>163</v>
@@ -4757,10 +4763,10 @@
         <v>213</v>
       </c>
       <c r="C119">
-        <v>86.734999999999999</v>
+        <v>79.8</v>
       </c>
       <c r="D119">
-        <v>87.28</v>
+        <v>80</v>
       </c>
       <c r="E119" t="s">
         <v>214</v>
@@ -4817,10 +4823,10 @@
         <v>219</v>
       </c>
       <c r="C122">
-        <v>87.66</v>
+        <v>82</v>
       </c>
       <c r="D122">
-        <v>87.82</v>
+        <v>83</v>
       </c>
       <c r="E122" t="s">
         <v>220</v>
@@ -4837,10 +4843,10 @@
         <v>221</v>
       </c>
       <c r="C123">
-        <v>87.82</v>
+        <v>82</v>
       </c>
       <c r="D123">
-        <v>87.83</v>
+        <v>83</v>
       </c>
       <c r="E123" t="s">
         <v>178</v>
@@ -4857,10 +4863,10 @@
         <v>222</v>
       </c>
       <c r="C124">
-        <v>87.83</v>
+        <v>82</v>
       </c>
       <c r="D124">
-        <v>87.83</v>
+        <v>83</v>
       </c>
       <c r="E124" t="s">
         <v>163</v>
@@ -4877,10 +4883,10 @@
         <v>223</v>
       </c>
       <c r="C125">
-        <v>87.83</v>
+        <v>82</v>
       </c>
       <c r="D125">
-        <v>87.844999999999999</v>
+        <v>83</v>
       </c>
       <c r="E125" t="s">
         <v>163</v>
@@ -4897,10 +4903,10 @@
         <v>224</v>
       </c>
       <c r="C126">
-        <v>87.844999999999999</v>
+        <v>83</v>
       </c>
       <c r="D126">
-        <v>89.33</v>
+        <v>84</v>
       </c>
       <c r="E126" t="s">
         <v>225</v>
@@ -4917,10 +4923,10 @@
         <v>226</v>
       </c>
       <c r="C127">
-        <v>89.33</v>
+        <v>86</v>
       </c>
       <c r="D127">
-        <v>89.46</v>
+        <v>87</v>
       </c>
       <c r="E127" t="s">
         <v>16</v>
@@ -4937,10 +4943,10 @@
         <v>227</v>
       </c>
       <c r="C128">
-        <v>89.46</v>
+        <v>87</v>
       </c>
       <c r="D128">
-        <v>89.49</v>
+        <v>88</v>
       </c>
       <c r="E128" t="s">
         <v>228</v>
@@ -4957,10 +4963,10 @@
         <v>229</v>
       </c>
       <c r="C129">
-        <v>89.49</v>
+        <v>87</v>
       </c>
       <c r="D129">
-        <v>89.49</v>
+        <v>88</v>
       </c>
       <c r="E129" t="s">
         <v>230</v>
@@ -4977,10 +4983,10 @@
         <v>231</v>
       </c>
       <c r="C130">
-        <v>89.49</v>
+        <v>87</v>
       </c>
       <c r="D130">
-        <v>89.6</v>
+        <v>88</v>
       </c>
       <c r="E130" t="s">
         <v>232</v>
@@ -4997,10 +5003,10 @@
         <v>233</v>
       </c>
       <c r="C131">
-        <v>89.6</v>
+        <v>88</v>
       </c>
       <c r="D131">
-        <v>90.66</v>
+        <v>89</v>
       </c>
       <c r="E131" t="s">
         <v>234</v>
@@ -5157,10 +5163,10 @@
         <v>245</v>
       </c>
       <c r="C139">
-        <v>92.01</v>
+        <v>90</v>
       </c>
       <c r="D139">
-        <v>93.234999999999999</v>
+        <v>91</v>
       </c>
       <c r="E139" t="s">
         <v>246</v>
@@ -5257,10 +5263,10 @@
         <v>252</v>
       </c>
       <c r="C144">
-        <v>96.034999999999997</v>
+        <v>92</v>
       </c>
       <c r="D144">
-        <v>96.034999999999997</v>
+        <v>93</v>
       </c>
       <c r="E144" t="s">
         <v>253</v>
@@ -5277,10 +5283,10 @@
         <v>254</v>
       </c>
       <c r="C145">
-        <v>96.034999999999997</v>
+        <v>93</v>
       </c>
       <c r="D145">
-        <v>96.614999999999995</v>
+        <v>94</v>
       </c>
       <c r="E145" t="s">
         <v>255</v>
@@ -5299,8 +5305,8 @@
       <c r="C146">
         <v>96.614999999999995</v>
       </c>
-      <c r="D146">
-        <v>96.734999999999999</v>
+      <c r="D146" t="s">
+        <v>495</v>
       </c>
       <c r="E146" t="s">
         <v>257</v>
@@ -5317,7 +5323,7 @@
         <v>258</v>
       </c>
       <c r="C147">
-        <v>96.734999999999999</v>
+        <v>95</v>
       </c>
       <c r="D147">
         <v>96.864999999999995</v>
@@ -5337,10 +5343,10 @@
         <v>259</v>
       </c>
       <c r="C148">
+        <v>95</v>
+      </c>
+      <c r="D148">
         <v>96.864999999999995</v>
-      </c>
-      <c r="D148">
-        <v>97.084999999999994</v>
       </c>
       <c r="E148" t="s">
         <v>260</v>
@@ -5357,10 +5363,10 @@
         <v>261</v>
       </c>
       <c r="C149">
-        <v>97.084999999999994</v>
+        <v>95</v>
       </c>
       <c r="D149">
-        <v>97.135000000000005</v>
+        <v>96.864999999999995</v>
       </c>
       <c r="E149" t="s">
         <v>25</v>
@@ -5377,10 +5383,10 @@
         <v>262</v>
       </c>
       <c r="C150">
-        <v>97.135000000000005</v>
+        <v>97</v>
       </c>
       <c r="D150">
-        <v>97.394999999999996</v>
+        <v>100</v>
       </c>
       <c r="E150" t="s">
         <v>263</v>
@@ -5397,10 +5403,10 @@
         <v>264</v>
       </c>
       <c r="C151">
-        <v>97.394999999999996</v>
+        <v>97</v>
       </c>
       <c r="D151">
-        <v>97.515000000000001</v>
+        <v>100</v>
       </c>
       <c r="E151" t="s">
         <v>263</v>
@@ -5417,7 +5423,7 @@
         <v>265</v>
       </c>
       <c r="C152">
-        <v>97.515000000000001</v>
+        <v>97</v>
       </c>
       <c r="D152">
         <v>98.57</v>
@@ -5477,10 +5483,10 @@
         <v>270</v>
       </c>
       <c r="C155">
-        <v>98.65</v>
+        <v>99</v>
       </c>
       <c r="D155">
-        <v>98.88</v>
+        <v>100</v>
       </c>
       <c r="E155" t="s">
         <v>271</v>
@@ -5497,10 +5503,10 @@
         <v>272</v>
       </c>
       <c r="C156">
-        <v>98.88</v>
+        <v>100</v>
       </c>
       <c r="D156">
-        <v>100.36</v>
+        <v>101</v>
       </c>
       <c r="E156" t="s">
         <v>273</v>
@@ -5517,10 +5523,10 @@
         <v>274</v>
       </c>
       <c r="C157">
-        <v>100.36</v>
+        <v>100</v>
       </c>
       <c r="D157">
-        <v>100.76</v>
+        <v>101</v>
       </c>
       <c r="E157" t="s">
         <v>275</v>
@@ -5537,10 +5543,10 @@
         <v>276</v>
       </c>
       <c r="C158">
-        <v>100.76</v>
+        <v>100</v>
       </c>
       <c r="D158">
-        <v>100.82</v>
+        <v>101</v>
       </c>
       <c r="E158" t="s">
         <v>277</v>
@@ -5657,7 +5663,7 @@
         <v>286</v>
       </c>
       <c r="C164">
-        <v>103.925</v>
+        <v>105.925</v>
       </c>
       <c r="D164">
         <v>107.27</v>
@@ -6397,10 +6403,10 @@
         <v>348</v>
       </c>
       <c r="C201">
-        <v>131.29</v>
+        <v>132.34</v>
       </c>
       <c r="D201">
-        <v>132.34</v>
+        <v>134.44999999999999</v>
       </c>
       <c r="E201" t="s">
         <v>349</v>
@@ -6506,7 +6512,7 @@
         <v>359</v>
       </c>
       <c r="F206" t="s">
-        <v>34</v>
+        <v>495</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -7199,8 +7205,8 @@
       <c r="C241">
         <v>166.96</v>
       </c>
-      <c r="D241">
-        <v>166.965</v>
+      <c r="D241" t="s">
+        <v>495</v>
       </c>
       <c r="E241" t="s">
         <v>196</v>
@@ -7220,7 +7226,7 @@
         <v>166.965</v>
       </c>
       <c r="D242">
-        <v>166.965</v>
+        <v>167.245</v>
       </c>
       <c r="E242" t="s">
         <v>417</v>
@@ -7240,7 +7246,7 @@
         <v>166.965</v>
       </c>
       <c r="D243">
-        <v>166.965</v>
+        <v>167.245</v>
       </c>
       <c r="E243" t="s">
         <v>417</v>
@@ -7260,7 +7266,7 @@
         <v>166.965</v>
       </c>
       <c r="D244">
-        <v>166.965</v>
+        <v>167.245</v>
       </c>
       <c r="E244" t="s">
         <v>417</v>
@@ -7280,7 +7286,7 @@
         <v>166.965</v>
       </c>
       <c r="D245">
-        <v>166.965</v>
+        <v>167.245</v>
       </c>
       <c r="E245" t="s">
         <v>421</v>

</xml_diff>